<commit_message>
Fix register, best seller month
</commit_message>
<xml_diff>
--- a/Documentation/DS GIAO NHIEM VU DATN DHCQ KHOA 2019_13092023 (1).xlsx
+++ b/Documentation/DS GIAO NHIEM VU DATN DHCQ KHOA 2019_13092023 (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tot-Nghiep\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DoAnTotNghiep\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF46889B-A6B8-43ED-B76B-8E862DFB1045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61821DE-266A-4503-8714-82ACABC0C03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2355" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15750" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSSV du dieu kien DATN" sheetId="1" state="hidden" r:id="rId1"/>
@@ -36133,7 +36133,7 @@
       <c r="Z8" s="52"/>
       <c r="AA8" s="44"/>
     </row>
-    <row r="9" spans="1:27" ht="124.8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="265.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="51">
         <v>2</v>
       </c>
@@ -36182,7 +36182,7 @@
       <c r="Z9" s="52"/>
       <c r="AA9" s="44"/>
     </row>
-    <row r="10" spans="1:27" ht="156" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="202.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="51">
         <v>3</v>
       </c>
@@ -36231,7 +36231,7 @@
       <c r="Z10" s="52"/>
       <c r="AA10" s="44"/>
     </row>
-    <row r="11" spans="1:27" ht="140.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="265.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="53">
         <v>4</v>
       </c>
@@ -36280,7 +36280,7 @@
       <c r="Z11" s="52"/>
       <c r="AA11" s="44"/>
     </row>
-    <row r="12" spans="1:27" ht="109.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="265.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="51">
         <v>5</v>
       </c>
@@ -36329,7 +36329,7 @@
       <c r="Z12" s="52"/>
       <c r="AA12" s="44"/>
     </row>
-    <row r="13" spans="1:27" ht="125.4" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" ht="265.8" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="51">
         <v>6</v>
       </c>
@@ -36378,7 +36378,7 @@
       <c r="Z13" s="52"/>
       <c r="AA13" s="44"/>
     </row>
-    <row r="14" spans="1:27" ht="109.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="265.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="51">
         <v>7</v>
       </c>
@@ -36427,7 +36427,7 @@
       <c r="Z14" s="52"/>
       <c r="AA14" s="44"/>
     </row>
-    <row r="15" spans="1:27" ht="140.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="202.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="51">
         <v>8</v>
       </c>
@@ -36574,7 +36574,7 @@
       <c r="Z17" s="52"/>
       <c r="AA17" s="44"/>
     </row>
-    <row r="18" spans="1:27" ht="171.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="187.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="51">
         <v>11</v>
       </c>
@@ -36623,7 +36623,7 @@
       <c r="Z18" s="52"/>
       <c r="AA18" s="44"/>
     </row>
-    <row r="19" spans="1:27" ht="156" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="218.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="51">
         <v>12</v>
       </c>
@@ -36721,7 +36721,7 @@
       <c r="Z20" s="52"/>
       <c r="AA20" s="44"/>
     </row>
-    <row r="21" spans="1:27" ht="78" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="218.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="51">
         <v>14</v>
       </c>
@@ -36921,7 +36921,7 @@
       <c r="Z24" s="52"/>
       <c r="AA24" s="44"/>
     </row>
-    <row r="25" spans="1:27" ht="156" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" ht="218.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="51">
         <v>18</v>
       </c>
@@ -36970,7 +36970,7 @@
       <c r="Z25" s="52"/>
       <c r="AA25" s="44"/>
     </row>
-    <row r="26" spans="1:27" ht="171.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" ht="187.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="51">
         <v>19</v>
       </c>
@@ -37019,7 +37019,7 @@
       <c r="Z26" s="54"/>
       <c r="AA26" s="54"/>
     </row>
-    <row r="27" spans="1:27" ht="265.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" ht="249.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="51">
         <v>20</v>
       </c>
@@ -37068,7 +37068,7 @@
       <c r="Z27" s="56"/>
       <c r="AA27" s="56"/>
     </row>
-    <row r="28" spans="1:27" ht="109.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" ht="234" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="51">
         <v>21</v>
       </c>
@@ -37117,7 +37117,7 @@
       <c r="Z28" s="57"/>
       <c r="AA28" s="57"/>
     </row>
-    <row r="29" spans="1:27" ht="109.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" ht="234" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="51">
         <v>22</v>
       </c>
@@ -37166,7 +37166,7 @@
       <c r="Z29" s="57"/>
       <c r="AA29" s="57"/>
     </row>
-    <row r="30" spans="1:27" ht="109.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" ht="234" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="51">
         <v>23</v>
       </c>
@@ -37215,7 +37215,7 @@
       <c r="Z30" s="57"/>
       <c r="AA30" s="57"/>
     </row>
-    <row r="31" spans="1:27" ht="109.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" ht="234" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="51">
         <v>24</v>
       </c>
@@ -37264,7 +37264,7 @@
       <c r="Z31" s="57"/>
       <c r="AA31" s="57"/>
     </row>
-    <row r="32" spans="1:27" ht="109.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" ht="234" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="51">
         <v>25</v>
       </c>
@@ -37313,7 +37313,7 @@
       <c r="Z32" s="57"/>
       <c r="AA32" s="57"/>
     </row>
-    <row r="33" spans="1:27" ht="171.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" ht="265.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="51">
         <v>26</v>
       </c>
@@ -37366,7 +37366,7 @@
       <c r="Z33" s="57"/>
       <c r="AA33" s="57"/>
     </row>
-    <row r="34" spans="1:27" ht="78" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" ht="249.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="51">
         <v>27</v>
       </c>
@@ -37415,7 +37415,7 @@
       <c r="Z34" s="57"/>
       <c r="AA34" s="57"/>
     </row>
-    <row r="35" spans="1:27" ht="93.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" ht="249.6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="51">
         <v>28</v>
       </c>
@@ -37464,7 +37464,7 @@
       <c r="Z35" s="44"/>
       <c r="AA35" s="44"/>
     </row>
-    <row r="36" spans="1:27" ht="109.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" ht="218.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="51">
         <v>29</v>
       </c>
@@ -37513,7 +37513,7 @@
       <c r="Z36" s="44"/>
       <c r="AA36" s="44"/>
     </row>
-    <row r="37" spans="1:27" ht="93.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" ht="218.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="51">
         <v>30</v>
       </c>
@@ -37562,7 +37562,7 @@
       <c r="Z37" s="44"/>
       <c r="AA37" s="44"/>
     </row>
-    <row r="38" spans="1:27" ht="140.4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" ht="218.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="51">
         <v>31</v>
       </c>
@@ -37611,7 +37611,7 @@
       <c r="Z38" s="44"/>
       <c r="AA38" s="44"/>
     </row>
-    <row r="39" spans="1:27" ht="109.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" ht="218.4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="51">
         <v>32</v>
       </c>
@@ -37709,7 +37709,7 @@
       <c r="Z40" s="44"/>
       <c r="AA40" s="44"/>
     </row>
-    <row r="41" spans="1:27" ht="171.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" ht="202.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="51">
         <v>34</v>
       </c>
@@ -37807,7 +37807,7 @@
       <c r="Z42" s="44"/>
       <c r="AA42" s="44"/>
     </row>
-    <row r="43" spans="1:27" ht="109.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" ht="202.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="51">
         <v>36</v>
       </c>
@@ -37954,7 +37954,7 @@
       <c r="Z45" s="44"/>
       <c r="AA45" s="44"/>
     </row>
-    <row r="46" spans="1:27" ht="171.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" ht="265.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="51">
         <v>39</v>
       </c>
@@ -38054,7 +38054,7 @@
       <c r="Z47" s="44"/>
       <c r="AA47" s="44"/>
     </row>
-    <row r="48" spans="1:27" ht="78" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" ht="202.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="51">
         <v>41</v>
       </c>
@@ -38250,7 +38250,7 @@
       <c r="Z51" s="44"/>
       <c r="AA51" s="44"/>
     </row>
-    <row r="52" spans="1:27" ht="78" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" ht="296.39999999999998" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="51">
         <v>46</v>
       </c>
@@ -38299,7 +38299,7 @@
       <c r="Z52" s="44"/>
       <c r="AA52" s="44"/>
     </row>
-    <row r="53" spans="1:27" ht="78" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" ht="296.39999999999998" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="51">
         <v>47</v>
       </c>
@@ -38348,7 +38348,7 @@
       <c r="Z53" s="44"/>
       <c r="AA53" s="44"/>
     </row>
-    <row r="54" spans="1:27" ht="109.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" ht="265.2" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="51">
         <v>48</v>
       </c>
@@ -38401,7 +38401,7 @@
       <c r="Z54" s="44"/>
       <c r="AA54" s="44"/>
     </row>
-    <row r="55" spans="1:27" ht="78" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" ht="296.39999999999998" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="51">
         <v>49</v>
       </c>
@@ -38597,7 +38597,7 @@
       <c r="Z58" s="44"/>
       <c r="AA58" s="44"/>
     </row>
-    <row r="59" spans="1:27" ht="93.6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" ht="202.8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="51">
         <v>53</v>
       </c>
@@ -45577,7 +45577,7 @@
       <c r="Z10" s="52"/>
       <c r="AA10" s="44"/>
     </row>
-    <row r="11" spans="1:27" ht="140.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="124.8" x14ac:dyDescent="0.25">
       <c r="A11" s="94">
         <v>4</v>
       </c>

</xml_diff>